<commit_message>
Integrate dynamic directory, profiles, navigation, and deployment config
</commit_message>
<xml_diff>
--- a/London muslim owned buisnesses.xlsx
+++ b/London muslim owned buisnesses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rabia\Documents\trae_projects\muslim women magazine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E08109A5-2DB9-451E-8315-91CE66509934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4628C5A3-8E02-4E31-8A08-86AF78D5B576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="565">
   <si>
     <t>Description / Speciality</t>
   </si>
@@ -1445,9 +1445,6 @@
     <t>Muslim-women-led adventure &amp; travel group for hijabis</t>
   </si>
   <si>
-    <t>Muslim-women-led hiking &amp; outdoor adventures</t>
-  </si>
-  <si>
     <t>Muslimah Adventures UK</t>
   </si>
   <si>
@@ -1566,9 +1563,6 @@
   </si>
   <si>
     <t xml:space="preserve"> @hijabiexplorersuk</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> @sistershikinggroupuk</t>
   </si>
   <si>
     <t xml:space="preserve"> @muslimahadventuresuk</t>
@@ -2102,6 +2096,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_GPT</we:customFunctionIds>
@@ -2139,6 +2136,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_AI_TABLE</we:customFunctionIds>
@@ -2169,10 +2169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A68B465C-0DD4-4434-AD8D-C7FB86C99943}">
-  <dimension ref="A1:I259"/>
+  <dimension ref="A1:I210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2189,7 +2189,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -2204,12 +2204,12 @@
         <v>44</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -2224,12 +2224,12 @@
         <v>45</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -2244,12 +2244,12 @@
         <v>45</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -2264,12 +2264,12 @@
         <v>45</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -2284,12 +2284,12 @@
         <v>46</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -2304,12 +2304,12 @@
         <v>47</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -2324,12 +2324,12 @@
         <v>48</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -2344,12 +2344,12 @@
         <v>45</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -2364,12 +2364,12 @@
         <v>49</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -2384,12 +2384,12 @@
         <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
@@ -2404,12 +2404,12 @@
         <v>50</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
@@ -2424,12 +2424,12 @@
         <v>49</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -2444,12 +2444,12 @@
         <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -2464,12 +2464,12 @@
         <v>51</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -2484,12 +2484,12 @@
         <v>52</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -2504,12 +2504,12 @@
         <v>45</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -2524,12 +2524,12 @@
         <v>53</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -2544,12 +2544,12 @@
         <v>51</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
@@ -2564,12 +2564,12 @@
         <v>52</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B20" t="s">
         <v>70</v>
@@ -2584,12 +2584,12 @@
         <v>48</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B21" t="s">
         <v>72</v>
@@ -2604,12 +2604,12 @@
         <v>75</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B22" t="s">
         <v>76</v>
@@ -2624,12 +2624,12 @@
         <v>75</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B23" t="s">
         <v>79</v>
@@ -2644,12 +2644,12 @@
         <v>82</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B24" t="s">
         <v>83</v>
@@ -2664,12 +2664,12 @@
         <v>75</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B25" t="s">
         <v>86</v>
@@ -2684,12 +2684,12 @@
         <v>75</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B26" t="s">
         <v>88</v>
@@ -2704,12 +2704,12 @@
         <v>75</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B27" t="s">
         <v>91</v>
@@ -2724,12 +2724,12 @@
         <v>75</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B28" t="s">
         <v>94</v>
@@ -2744,12 +2744,12 @@
         <v>75</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B29" t="s">
         <v>96</v>
@@ -2764,12 +2764,12 @@
         <v>75</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B30" t="s">
         <v>99</v>
@@ -2784,12 +2784,12 @@
         <v>101</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B31" t="s">
         <v>102</v>
@@ -2804,12 +2804,12 @@
         <v>48</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B32" t="s">
         <v>105</v>
@@ -2824,12 +2824,12 @@
         <v>108</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B33" t="s">
         <v>109</v>
@@ -2844,12 +2844,12 @@
         <v>112</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B34" t="s">
         <v>113</v>
@@ -2864,12 +2864,12 @@
         <v>116</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B35" t="s">
         <v>117</v>
@@ -2884,12 +2884,12 @@
         <v>119</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B36" t="s">
         <v>120</v>
@@ -2904,12 +2904,12 @@
         <v>116</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B37" t="s">
         <v>123</v>
@@ -2924,12 +2924,12 @@
         <v>119</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B38" t="s">
         <v>126</v>
@@ -2944,12 +2944,12 @@
         <v>119</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B39" t="s">
         <v>128</v>
@@ -2964,12 +2964,12 @@
         <v>119</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B40" t="s">
         <v>130</v>
@@ -2984,12 +2984,12 @@
         <v>119</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B41" t="s">
         <v>440</v>
@@ -3001,12 +3001,12 @@
         <v>442</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B42" t="s">
         <v>443</v>
@@ -3018,12 +3018,12 @@
         <v>413</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B43" t="s">
         <v>406</v>
@@ -3035,12 +3035,12 @@
         <v>421</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B44" t="s">
         <v>408</v>
@@ -3052,12 +3052,12 @@
         <v>409</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B45" t="s">
         <v>410</v>
@@ -3069,12 +3069,12 @@
         <v>411</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B46" t="s">
         <v>412</v>
@@ -3086,12 +3086,12 @@
         <v>424</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B47" t="s">
         <v>414</v>
@@ -3103,12 +3103,12 @@
         <v>415</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B48" t="s">
         <v>416</v>
@@ -3120,12 +3120,12 @@
         <v>417</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B49" t="s">
         <v>418</v>
@@ -3137,12 +3137,12 @@
         <v>419</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B50" t="s">
         <v>420</v>
@@ -3154,12 +3154,12 @@
         <v>452</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B51" t="s">
         <v>422</v>
@@ -3171,12 +3171,12 @@
         <v>424</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B52" t="s">
         <v>425</v>
@@ -3188,12 +3188,12 @@
         <v>426</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B53" t="s">
         <v>427</v>
@@ -3205,12 +3205,12 @@
         <v>428</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B54" t="s">
         <v>429</v>
@@ -3222,12 +3222,12 @@
         <v>409</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B55" t="s">
         <v>430</v>
@@ -3239,12 +3239,12 @@
         <v>424</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B56" t="s">
         <v>432</v>
@@ -3256,12 +3256,12 @@
         <v>411</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B57" t="s">
         <v>433</v>
@@ -3273,12 +3273,12 @@
         <v>424</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B58" t="s">
         <v>434</v>
@@ -3290,12 +3290,12 @@
         <v>417</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B59" t="s">
         <v>435</v>
@@ -3307,12 +3307,12 @@
         <v>436</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="B60" t="s">
         <v>437</v>
@@ -3324,41 +3324,41 @@
         <v>439</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B61" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C61" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D61" t="s">
         <v>1</v>
       </c>
       <c r="E61" t="s">
+        <v>530</v>
+      </c>
+      <c r="F61" t="s">
+        <v>531</v>
+      </c>
+      <c r="G61" t="s">
         <v>532</v>
       </c>
-      <c r="F61" t="s">
+      <c r="H61" t="s">
         <v>533</v>
       </c>
-      <c r="G61" t="s">
+      <c r="I61" t="s">
         <v>534</v>
-      </c>
-      <c r="H61" t="s">
-        <v>535</v>
-      </c>
-      <c r="I61" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B62" t="s">
         <v>309</v>
@@ -3375,7 +3375,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B63" t="s">
         <v>312</v>
@@ -3392,7 +3392,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B64" t="s">
         <v>314</v>
@@ -3409,7 +3409,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B65" t="s">
         <v>316</v>
@@ -3426,7 +3426,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B66" t="s">
         <v>319</v>
@@ -3443,7 +3443,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B67" t="s">
         <v>321</v>
@@ -3460,7 +3460,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B68" t="s">
         <v>323</v>
@@ -3477,7 +3477,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B69" t="s">
         <v>325</v>
@@ -3494,7 +3494,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B70" t="s">
         <v>327</v>
@@ -3511,7 +3511,7 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B71" t="s">
         <v>329</v>
@@ -3528,7 +3528,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B72" t="s">
         <v>331</v>
@@ -3545,7 +3545,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B73" t="s">
         <v>333</v>
@@ -3562,7 +3562,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B74" t="s">
         <v>335</v>
@@ -3579,7 +3579,7 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B75" t="s">
         <v>337</v>
@@ -3596,7 +3596,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B76" t="s">
         <v>339</v>
@@ -3613,7 +3613,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B77" t="s">
         <v>341</v>
@@ -3630,7 +3630,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B78" t="s">
         <v>343</v>
@@ -3647,7 +3647,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B79" t="s">
         <v>345</v>
@@ -3664,7 +3664,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B80" t="s">
         <v>347</v>
@@ -3681,7 +3681,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B81" t="s">
         <v>349</v>
@@ -3698,7 +3698,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B82" t="s">
         <v>352</v>
@@ -3715,7 +3715,7 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B83" t="s">
         <v>354</v>
@@ -3732,7 +3732,7 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B84" t="s">
         <v>356</v>
@@ -3749,7 +3749,7 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B85" t="s">
         <v>358</v>
@@ -3766,7 +3766,7 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B86" t="s">
         <v>360</v>
@@ -3783,7 +3783,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B87" t="s">
         <v>362</v>
@@ -3800,7 +3800,7 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B88" t="s">
         <v>364</v>
@@ -3817,7 +3817,7 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B89" t="s">
         <v>366</v>
@@ -3834,7 +3834,7 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B90" t="s">
         <v>370</v>
@@ -3851,7 +3851,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B91" t="s">
         <v>372</v>
@@ -3868,7 +3868,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B92" t="s">
         <v>375</v>
@@ -3885,7 +3885,7 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B93" t="s">
         <v>378</v>
@@ -3902,7 +3902,7 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B94" t="s">
         <v>381</v>
@@ -3919,7 +3919,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B95" t="s">
         <v>383</v>
@@ -3936,7 +3936,7 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B96" t="s">
         <v>386</v>
@@ -3953,7 +3953,7 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B97" t="s">
         <v>388</v>
@@ -3970,7 +3970,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B98" t="s">
         <v>390</v>
@@ -3987,7 +3987,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B99" t="s">
         <v>392</v>
@@ -4004,7 +4004,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B100" t="s">
         <v>394</v>
@@ -4021,7 +4021,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B101" t="s">
         <v>396</v>
@@ -4038,7 +4038,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B102" t="s">
         <v>398</v>
@@ -4055,7 +4055,7 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B103" t="s">
         <v>400</v>
@@ -4072,7 +4072,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B104" t="s">
         <v>402</v>
@@ -4089,7 +4089,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B105" t="s">
         <v>404</v>
@@ -4106,7 +4106,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B106" t="s">
         <v>54</v>
@@ -4121,12 +4121,12 @@
         <v>47</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B107" t="s">
         <v>55</v>
@@ -4141,12 +4141,12 @@
         <v>48</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B108" t="s">
         <v>56</v>
@@ -4161,12 +4161,12 @@
         <v>45</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B109" t="s">
         <v>57</v>
@@ -4181,12 +4181,12 @@
         <v>45</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B110" t="s">
         <v>58</v>
@@ -4201,12 +4201,12 @@
         <v>138</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B111" t="s">
         <v>59</v>
@@ -4221,12 +4221,12 @@
         <v>45</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B112" t="s">
         <v>60</v>
@@ -4241,12 +4241,12 @@
         <v>45</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B113" t="s">
         <v>61</v>
@@ -4261,12 +4261,12 @@
         <v>45</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B114" t="s">
         <v>62</v>
@@ -4281,12 +4281,12 @@
         <v>52</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B115" t="s">
         <v>63</v>
@@ -4301,12 +4301,12 @@
         <v>52</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B116" t="s">
         <v>64</v>
@@ -4324,7 +4324,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B117" t="s">
         <v>65</v>
@@ -4342,7 +4342,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B118" t="s">
         <v>66</v>
@@ -4360,7 +4360,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B119" t="s">
         <v>67</v>
@@ -4378,7 +4378,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B120" t="s">
         <v>68</v>
@@ -4396,7 +4396,7 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B121" t="s">
         <v>69</v>
@@ -4414,7 +4414,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B122" t="s">
         <v>150</v>
@@ -4431,7 +4431,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B123" t="s">
         <v>153</v>
@@ -4448,7 +4448,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B124" t="s">
         <v>155</v>
@@ -4465,7 +4465,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B125" t="s">
         <v>157</v>
@@ -4482,7 +4482,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B126" t="s">
         <v>159</v>
@@ -4499,7 +4499,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B127" t="s">
         <v>161</v>
@@ -4516,7 +4516,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B128" t="s">
         <v>164</v>
@@ -4533,7 +4533,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B129" t="s">
         <v>168</v>
@@ -4550,7 +4550,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B130" t="s">
         <v>170</v>
@@ -4567,7 +4567,7 @@
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B131" t="s">
         <v>172</v>
@@ -4584,7 +4584,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B132" t="s">
         <v>174</v>
@@ -4601,7 +4601,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B133" t="s">
         <v>177</v>
@@ -4618,7 +4618,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B134" t="s">
         <v>179</v>
@@ -4635,7 +4635,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B135" t="s">
         <v>182</v>
@@ -4652,7 +4652,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B136" t="s">
         <v>185</v>
@@ -4669,7 +4669,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B137" t="s">
         <v>188</v>
@@ -4686,7 +4686,7 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B138" t="s">
         <v>191</v>
@@ -4703,118 +4703,118 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B139" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C139" t="s">
-        <v>353</v>
+        <v>0</v>
       </c>
       <c r="D139" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="E139" t="s">
-        <v>45</v>
+        <v>194</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B140" t="s">
-        <v>354</v>
+        <v>195</v>
       </c>
       <c r="C140" t="s">
-        <v>355</v>
+        <v>196</v>
       </c>
       <c r="D140" t="s">
-        <v>40</v>
+        <v>197</v>
       </c>
       <c r="E140" t="s">
-        <v>45</v>
+        <v>198</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B141" t="s">
-        <v>356</v>
+        <v>199</v>
       </c>
       <c r="C141" t="s">
-        <v>357</v>
+        <v>200</v>
       </c>
       <c r="D141" t="s">
-        <v>41</v>
+        <v>201</v>
       </c>
       <c r="E141" t="s">
-        <v>45</v>
+        <v>202</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B142" t="s">
-        <v>358</v>
+        <v>203</v>
       </c>
       <c r="C142" t="s">
-        <v>359</v>
+        <v>204</v>
       </c>
       <c r="D142" t="s">
-        <v>40</v>
+        <v>197</v>
       </c>
       <c r="E142" t="s">
-        <v>45</v>
+        <v>202</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B143" t="s">
-        <v>360</v>
+        <v>205</v>
       </c>
       <c r="C143" t="s">
-        <v>361</v>
+        <v>206</v>
       </c>
       <c r="D143" t="s">
-        <v>40</v>
+        <v>197</v>
       </c>
       <c r="E143" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B144" t="s">
-        <v>362</v>
+        <v>207</v>
       </c>
       <c r="C144" t="s">
-        <v>363</v>
+        <v>208</v>
       </c>
       <c r="D144" t="s">
-        <v>40</v>
+        <v>209</v>
       </c>
       <c r="E144" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B145" t="s">
-        <v>364</v>
+        <v>210</v>
       </c>
       <c r="C145" t="s">
-        <v>365</v>
+        <v>211</v>
       </c>
       <c r="D145" t="s">
-        <v>40</v>
+        <v>212</v>
       </c>
       <c r="E145" t="s">
         <v>101</v>
@@ -4822,33 +4822,33 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B146" t="s">
-        <v>366</v>
+        <v>213</v>
       </c>
       <c r="C146" t="s">
-        <v>367</v>
+        <v>214</v>
       </c>
       <c r="D146" t="s">
-        <v>368</v>
+        <v>215</v>
       </c>
       <c r="E146" t="s">
-        <v>369</v>
+        <v>101</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B147" t="s">
-        <v>370</v>
+        <v>216</v>
       </c>
       <c r="C147" t="s">
-        <v>371</v>
+        <v>217</v>
       </c>
       <c r="D147" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="E147" t="s">
         <v>101</v>
@@ -4856,33 +4856,33 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B148" t="s">
-        <v>372</v>
+        <v>219</v>
       </c>
       <c r="C148" t="s">
-        <v>373</v>
+        <v>220</v>
       </c>
       <c r="D148" t="s">
-        <v>374</v>
+        <v>218</v>
       </c>
       <c r="E148" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B149" t="s">
-        <v>375</v>
+        <v>221</v>
       </c>
       <c r="C149" t="s">
-        <v>376</v>
+        <v>222</v>
       </c>
       <c r="D149" t="s">
-        <v>377</v>
+        <v>223</v>
       </c>
       <c r="E149" t="s">
         <v>101</v>
@@ -4890,16 +4890,16 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B150" t="s">
-        <v>378</v>
+        <v>224</v>
       </c>
       <c r="C150" t="s">
-        <v>379</v>
+        <v>285</v>
       </c>
       <c r="D150" t="s">
-        <v>380</v>
+        <v>225</v>
       </c>
       <c r="E150" t="s">
         <v>101</v>
@@ -4907,16 +4907,16 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B151" t="s">
-        <v>381</v>
+        <v>226</v>
       </c>
       <c r="C151" t="s">
-        <v>382</v>
+        <v>227</v>
       </c>
       <c r="D151" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E151" t="s">
         <v>101</v>
@@ -4924,16 +4924,16 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B152" t="s">
-        <v>383</v>
+        <v>229</v>
       </c>
       <c r="C152" t="s">
-        <v>384</v>
+        <v>230</v>
       </c>
       <c r="D152" t="s">
-        <v>385</v>
+        <v>228</v>
       </c>
       <c r="E152" t="s">
         <v>101</v>
@@ -4941,50 +4941,50 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B153" t="s">
-        <v>386</v>
+        <v>231</v>
       </c>
       <c r="C153" t="s">
-        <v>387</v>
+        <v>232</v>
       </c>
       <c r="D153" t="s">
-        <v>40</v>
+        <v>228</v>
       </c>
       <c r="E153" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B154" t="s">
-        <v>388</v>
+        <v>233</v>
       </c>
       <c r="C154" t="s">
-        <v>389</v>
+        <v>232</v>
       </c>
       <c r="D154" t="s">
-        <v>40</v>
+        <v>228</v>
       </c>
       <c r="E154" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B155" t="s">
-        <v>390</v>
+        <v>234</v>
       </c>
       <c r="C155" t="s">
-        <v>391</v>
+        <v>235</v>
       </c>
       <c r="D155" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E155" t="s">
         <v>45</v>
@@ -4992,16 +4992,16 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B156" t="s">
-        <v>392</v>
+        <v>236</v>
       </c>
       <c r="C156" t="s">
-        <v>393</v>
+        <v>237</v>
       </c>
       <c r="D156" t="s">
-        <v>40</v>
+        <v>238</v>
       </c>
       <c r="E156" t="s">
         <v>45</v>
@@ -5009,237 +5009,237 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B157" t="s">
-        <v>394</v>
+        <v>239</v>
       </c>
       <c r="C157" t="s">
-        <v>395</v>
+        <v>240</v>
       </c>
       <c r="D157" t="s">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="E157" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B158" t="s">
-        <v>396</v>
+        <v>241</v>
       </c>
       <c r="C158" t="s">
-        <v>397</v>
+        <v>220</v>
       </c>
       <c r="D158" t="s">
-        <v>40</v>
+        <v>242</v>
       </c>
       <c r="E158" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B159" t="s">
-        <v>398</v>
+        <v>243</v>
       </c>
       <c r="C159" t="s">
-        <v>399</v>
+        <v>244</v>
       </c>
       <c r="D159" t="s">
-        <v>40</v>
+        <v>245</v>
       </c>
       <c r="E159" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B160" t="s">
-        <v>400</v>
+        <v>246</v>
       </c>
       <c r="C160" t="s">
-        <v>401</v>
+        <v>247</v>
       </c>
       <c r="D160" t="s">
-        <v>40</v>
+        <v>245</v>
       </c>
       <c r="E160" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B161" t="s">
-        <v>402</v>
+        <v>248</v>
       </c>
       <c r="C161" t="s">
-        <v>403</v>
+        <v>249</v>
       </c>
       <c r="D161" t="s">
-        <v>40</v>
+        <v>197</v>
       </c>
       <c r="E161" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B162" t="s">
-        <v>404</v>
+        <v>250</v>
       </c>
       <c r="C162" t="s">
-        <v>405</v>
+        <v>251</v>
       </c>
       <c r="D162" t="s">
-        <v>368</v>
+        <v>252</v>
       </c>
       <c r="E162" t="s">
-        <v>369</v>
+        <v>101</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B163" t="s">
-        <v>351</v>
+        <v>253</v>
       </c>
       <c r="C163" t="s">
-        <v>0</v>
+        <v>251</v>
       </c>
       <c r="D163" t="s">
-        <v>1</v>
+        <v>252</v>
       </c>
       <c r="E163" t="s">
-        <v>194</v>
+        <v>119</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B164" t="s">
-        <v>352</v>
+        <v>254</v>
       </c>
       <c r="C164" t="s">
-        <v>353</v>
+        <v>255</v>
       </c>
       <c r="D164" t="s">
-        <v>40</v>
+        <v>197</v>
       </c>
       <c r="E164" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B165" t="s">
-        <v>354</v>
+        <v>256</v>
       </c>
       <c r="C165" t="s">
-        <v>355</v>
+        <v>257</v>
       </c>
       <c r="D165" t="s">
-        <v>40</v>
+        <v>245</v>
       </c>
       <c r="E165" t="s">
-        <v>45</v>
+        <v>119</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B166" t="s">
-        <v>356</v>
+        <v>258</v>
       </c>
       <c r="C166" t="s">
-        <v>357</v>
+        <v>259</v>
       </c>
       <c r="D166" t="s">
-        <v>41</v>
+        <v>260</v>
       </c>
       <c r="E166" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B167" t="s">
-        <v>358</v>
+        <v>261</v>
       </c>
       <c r="C167" t="s">
-        <v>359</v>
+        <v>259</v>
       </c>
       <c r="D167" t="s">
-        <v>40</v>
+        <v>262</v>
       </c>
       <c r="E167" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B168" t="s">
-        <v>360</v>
+        <v>263</v>
       </c>
       <c r="C168" t="s">
-        <v>361</v>
+        <v>264</v>
       </c>
       <c r="D168" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E168" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B169" t="s">
-        <v>362</v>
+        <v>265</v>
       </c>
       <c r="C169" t="s">
-        <v>363</v>
+        <v>266</v>
       </c>
       <c r="D169" t="s">
-        <v>40</v>
+        <v>267</v>
       </c>
       <c r="E169" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B170" t="s">
-        <v>364</v>
+        <v>268</v>
       </c>
       <c r="C170" t="s">
-        <v>365</v>
+        <v>264</v>
       </c>
       <c r="D170" t="s">
-        <v>40</v>
+        <v>269</v>
       </c>
       <c r="E170" t="s">
         <v>101</v>
@@ -5247,50 +5247,50 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B171" t="s">
-        <v>366</v>
+        <v>270</v>
       </c>
       <c r="C171" t="s">
-        <v>367</v>
+        <v>271</v>
       </c>
       <c r="D171" t="s">
-        <v>368</v>
+        <v>272</v>
       </c>
       <c r="E171" t="s">
-        <v>369</v>
+        <v>101</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B172" t="s">
-        <v>370</v>
+        <v>273</v>
       </c>
       <c r="C172" t="s">
-        <v>371</v>
+        <v>274</v>
       </c>
       <c r="D172" t="s">
-        <v>197</v>
+        <v>41</v>
       </c>
       <c r="E172" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B173" t="s">
-        <v>372</v>
+        <v>275</v>
       </c>
       <c r="C173" t="s">
-        <v>373</v>
+        <v>286</v>
       </c>
       <c r="D173" t="s">
-        <v>374</v>
+        <v>276</v>
       </c>
       <c r="E173" t="s">
         <v>101</v>
@@ -5298,16 +5298,16 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B174" t="s">
-        <v>375</v>
+        <v>277</v>
       </c>
       <c r="C174" t="s">
-        <v>376</v>
+        <v>278</v>
       </c>
       <c r="D174" t="s">
-        <v>377</v>
+        <v>279</v>
       </c>
       <c r="E174" t="s">
         <v>101</v>
@@ -5315,1531 +5315,695 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B175" t="s">
-        <v>378</v>
+        <v>280</v>
       </c>
       <c r="C175" t="s">
-        <v>379</v>
+        <v>281</v>
       </c>
       <c r="D175" t="s">
-        <v>380</v>
+        <v>197</v>
       </c>
       <c r="E175" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B176" t="s">
-        <v>381</v>
+        <v>282</v>
       </c>
       <c r="C176" t="s">
-        <v>382</v>
+        <v>283</v>
       </c>
       <c r="D176" t="s">
-        <v>225</v>
+        <v>284</v>
       </c>
       <c r="E176" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B177" t="s">
-        <v>383</v>
+        <v>287</v>
       </c>
       <c r="C177" t="s">
-        <v>384</v>
+        <v>288</v>
       </c>
       <c r="D177" t="s">
-        <v>385</v>
+        <v>228</v>
       </c>
       <c r="E177" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B178" t="s">
-        <v>386</v>
+        <v>289</v>
       </c>
       <c r="C178" t="s">
-        <v>387</v>
+        <v>290</v>
       </c>
       <c r="D178" t="s">
-        <v>40</v>
+        <v>228</v>
       </c>
       <c r="E178" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B179" t="s">
-        <v>388</v>
+        <v>291</v>
       </c>
       <c r="C179" t="s">
-        <v>389</v>
+        <v>292</v>
       </c>
       <c r="D179" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E179" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B180" t="s">
-        <v>390</v>
+        <v>293</v>
       </c>
       <c r="C180" t="s">
-        <v>391</v>
+        <v>294</v>
       </c>
       <c r="D180" t="s">
-        <v>40</v>
+        <v>245</v>
       </c>
       <c r="E180" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B181" t="s">
-        <v>392</v>
+        <v>295</v>
       </c>
       <c r="C181" t="s">
-        <v>393</v>
+        <v>296</v>
       </c>
       <c r="D181" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E181" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B182" t="s">
-        <v>394</v>
+        <v>297</v>
       </c>
       <c r="C182" t="s">
-        <v>395</v>
+        <v>298</v>
       </c>
       <c r="D182" t="s">
-        <v>40</v>
+        <v>197</v>
       </c>
       <c r="E182" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B183" t="s">
-        <v>396</v>
+        <v>299</v>
       </c>
       <c r="C183" t="s">
-        <v>397</v>
+        <v>300</v>
       </c>
       <c r="D183" t="s">
-        <v>40</v>
+        <v>301</v>
       </c>
       <c r="E183" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B184" t="s">
-        <v>398</v>
+        <v>302</v>
       </c>
       <c r="C184" t="s">
-        <v>399</v>
+        <v>303</v>
       </c>
       <c r="D184" t="s">
-        <v>40</v>
+        <v>301</v>
       </c>
       <c r="E184" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B185" t="s">
-        <v>400</v>
+        <v>304</v>
       </c>
       <c r="C185" t="s">
-        <v>401</v>
+        <v>305</v>
       </c>
       <c r="D185" t="s">
-        <v>40</v>
+        <v>306</v>
       </c>
       <c r="E185" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B186" t="s">
-        <v>402</v>
+        <v>307</v>
       </c>
       <c r="C186" t="s">
-        <v>403</v>
+        <v>308</v>
       </c>
       <c r="D186" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E186" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
+        <v>526</v>
+      </c>
+      <c r="B187" t="s">
+        <v>460</v>
+      </c>
+      <c r="C187" t="s">
+        <v>461</v>
+      </c>
+      <c r="D187" t="s">
+        <v>527</v>
+      </c>
+      <c r="E187" t="s">
+        <v>40</v>
+      </c>
+      <c r="F187" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>526</v>
+      </c>
+      <c r="B188" t="s">
+        <v>462</v>
+      </c>
+      <c r="C188" t="s">
+        <v>463</v>
+      </c>
+      <c r="D188" t="s">
+        <v>527</v>
+      </c>
+      <c r="E188" t="s">
+        <v>40</v>
+      </c>
+      <c r="F188" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>526</v>
+      </c>
+      <c r="B189" t="s">
+        <v>464</v>
+      </c>
+      <c r="C189" t="s">
+        <v>465</v>
+      </c>
+      <c r="D189" t="s">
+        <v>527</v>
+      </c>
+      <c r="E189" t="s">
+        <v>40</v>
+      </c>
+      <c r="F189" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>526</v>
+      </c>
+      <c r="B190" t="s">
+        <v>466</v>
+      </c>
+      <c r="C190" t="s">
+        <v>467</v>
+      </c>
+      <c r="D190" t="s">
+        <v>527</v>
+      </c>
+      <c r="E190" t="s">
+        <v>40</v>
+      </c>
+      <c r="F190" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>526</v>
+      </c>
+      <c r="B191" t="s">
+        <v>468</v>
+      </c>
+      <c r="C191" t="s">
+        <v>469</v>
+      </c>
+      <c r="D191" t="s">
+        <v>527</v>
+      </c>
+      <c r="E191" t="s">
+        <v>40</v>
+      </c>
+      <c r="F191" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>526</v>
+      </c>
+      <c r="B192" t="s">
+        <v>470</v>
+      </c>
+      <c r="C192" t="s">
+        <v>471</v>
+      </c>
+      <c r="D192" t="s">
+        <v>527</v>
+      </c>
+      <c r="E192" t="s">
+        <v>40</v>
+      </c>
+      <c r="F192" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>526</v>
+      </c>
+      <c r="B193" t="s">
+        <v>472</v>
+      </c>
+      <c r="C193" t="s">
+        <v>473</v>
+      </c>
+      <c r="D193" t="s">
+        <v>527</v>
+      </c>
+      <c r="E193" t="s">
+        <v>40</v>
+      </c>
+      <c r="F193" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>526</v>
+      </c>
+      <c r="B194" t="s">
+        <v>474</v>
+      </c>
+      <c r="C194" t="s">
+        <v>475</v>
+      </c>
+      <c r="D194" t="s">
+        <v>527</v>
+      </c>
+      <c r="E194" t="s">
+        <v>40</v>
+      </c>
+      <c r="F194" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>526</v>
+      </c>
+      <c r="B195" t="s">
+        <v>476</v>
+      </c>
+      <c r="C195" t="s">
+        <v>477</v>
+      </c>
+      <c r="D195" t="s">
+        <v>527</v>
+      </c>
+      <c r="E195" t="s">
+        <v>40</v>
+      </c>
+      <c r="F195" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>526</v>
+      </c>
+      <c r="B196" t="s">
+        <v>478</v>
+      </c>
+      <c r="C196" t="s">
+        <v>479</v>
+      </c>
+      <c r="D196" t="s">
+        <v>527</v>
+      </c>
+      <c r="E196" t="s">
+        <v>40</v>
+      </c>
+      <c r="F196" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>526</v>
+      </c>
+      <c r="B197" t="s">
+        <v>480</v>
+      </c>
+      <c r="C197" t="s">
+        <v>481</v>
+      </c>
+      <c r="D197" t="s">
+        <v>527</v>
+      </c>
+      <c r="E197" t="s">
+        <v>40</v>
+      </c>
+      <c r="F197" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>526</v>
+      </c>
+      <c r="B198" t="s">
+        <v>482</v>
+      </c>
+      <c r="C198" t="s">
+        <v>483</v>
+      </c>
+      <c r="D198" t="s">
+        <v>527</v>
+      </c>
+      <c r="E198" t="s">
+        <v>40</v>
+      </c>
+      <c r="F198" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>526</v>
+      </c>
+      <c r="B199" t="s">
+        <v>484</v>
+      </c>
+      <c r="C199" t="s">
+        <v>485</v>
+      </c>
+      <c r="D199" t="s">
+        <v>527</v>
+      </c>
+      <c r="E199" t="s">
+        <v>40</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
+        <v>526</v>
+      </c>
+      <c r="B200" t="s">
+        <v>486</v>
+      </c>
+      <c r="C200" t="s">
+        <v>487</v>
+      </c>
+      <c r="D200" t="s">
+        <v>527</v>
+      </c>
+      <c r="E200" t="s">
+        <v>40</v>
+      </c>
+      <c r="F200" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
+        <v>526</v>
+      </c>
+      <c r="B201" t="s">
+        <v>488</v>
+      </c>
+      <c r="C201" t="s">
+        <v>489</v>
+      </c>
+      <c r="D201" t="s">
+        <v>527</v>
+      </c>
+      <c r="E201" t="s">
+        <v>40</v>
+      </c>
+      <c r="F201" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
+        <v>526</v>
+      </c>
+      <c r="B202" t="s">
+        <v>522</v>
+      </c>
+      <c r="C202" t="s">
+        <v>490</v>
+      </c>
+      <c r="D202" t="s">
+        <v>527</v>
+      </c>
+      <c r="E202" t="s">
+        <v>40</v>
+      </c>
+      <c r="F202" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="B187" t="s">
-        <v>404</v>
-      </c>
-      <c r="C187" t="s">
-        <v>405</v>
-      </c>
-      <c r="D187" t="s">
-        <v>368</v>
-      </c>
-      <c r="E187" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A188" t="s">
-        <v>539</v>
-      </c>
-      <c r="B188" t="s">
-        <v>195</v>
-      </c>
-      <c r="C188" t="s">
-        <v>196</v>
-      </c>
-      <c r="D188" t="s">
-        <v>197</v>
-      </c>
-      <c r="E188" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A189" t="s">
-        <v>539</v>
-      </c>
-      <c r="B189" t="s">
-        <v>199</v>
-      </c>
-      <c r="C189" t="s">
-        <v>200</v>
-      </c>
-      <c r="D189" t="s">
-        <v>201</v>
-      </c>
-      <c r="E189" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A190" t="s">
-        <v>539</v>
-      </c>
-      <c r="B190" t="s">
-        <v>203</v>
-      </c>
-      <c r="C190" t="s">
-        <v>204</v>
-      </c>
-      <c r="D190" t="s">
-        <v>197</v>
-      </c>
-      <c r="E190" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A191" t="s">
-        <v>539</v>
-      </c>
-      <c r="B191" t="s">
-        <v>205</v>
-      </c>
-      <c r="C191" t="s">
-        <v>206</v>
-      </c>
-      <c r="D191" t="s">
-        <v>197</v>
-      </c>
-      <c r="E191" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A192" t="s">
-        <v>539</v>
-      </c>
-      <c r="B192" t="s">
-        <v>207</v>
-      </c>
-      <c r="C192" t="s">
-        <v>208</v>
-      </c>
-      <c r="D192" t="s">
-        <v>209</v>
-      </c>
-      <c r="E192" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A193" t="s">
-        <v>539</v>
-      </c>
-      <c r="B193" t="s">
-        <v>210</v>
-      </c>
-      <c r="C193" t="s">
-        <v>211</v>
-      </c>
-      <c r="D193" t="s">
-        <v>212</v>
-      </c>
-      <c r="E193" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A194" t="s">
-        <v>539</v>
-      </c>
-      <c r="B194" t="s">
-        <v>213</v>
-      </c>
-      <c r="C194" t="s">
-        <v>214</v>
-      </c>
-      <c r="D194" t="s">
-        <v>215</v>
-      </c>
-      <c r="E194" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A195" t="s">
-        <v>539</v>
-      </c>
-      <c r="B195" t="s">
-        <v>216</v>
-      </c>
-      <c r="C195" t="s">
-        <v>217</v>
-      </c>
-      <c r="D195" t="s">
-        <v>218</v>
-      </c>
-      <c r="E195" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A196" t="s">
-        <v>539</v>
-      </c>
-      <c r="B196" t="s">
-        <v>219</v>
-      </c>
-      <c r="C196" t="s">
-        <v>220</v>
-      </c>
-      <c r="D196" t="s">
-        <v>218</v>
-      </c>
-      <c r="E196" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A197" t="s">
-        <v>539</v>
-      </c>
-      <c r="B197" t="s">
-        <v>221</v>
-      </c>
-      <c r="C197" t="s">
-        <v>222</v>
-      </c>
-      <c r="D197" t="s">
-        <v>223</v>
-      </c>
-      <c r="E197" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A198" t="s">
-        <v>539</v>
-      </c>
-      <c r="B198" t="s">
-        <v>224</v>
-      </c>
-      <c r="C198" t="s">
-        <v>285</v>
-      </c>
-      <c r="D198" t="s">
-        <v>225</v>
-      </c>
-      <c r="E198" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A199" t="s">
-        <v>539</v>
-      </c>
-      <c r="B199" t="s">
-        <v>226</v>
-      </c>
-      <c r="C199" t="s">
-        <v>227</v>
-      </c>
-      <c r="D199" t="s">
-        <v>228</v>
-      </c>
-      <c r="E199" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A200" t="s">
-        <v>539</v>
-      </c>
-      <c r="B200" t="s">
-        <v>229</v>
-      </c>
-      <c r="C200" t="s">
-        <v>230</v>
-      </c>
-      <c r="D200" t="s">
-        <v>228</v>
-      </c>
-      <c r="E200" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A201" t="s">
-        <v>539</v>
-      </c>
-      <c r="B201" t="s">
-        <v>231</v>
-      </c>
-      <c r="C201" t="s">
-        <v>232</v>
-      </c>
-      <c r="D201" t="s">
-        <v>228</v>
-      </c>
-      <c r="E201" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A202" t="s">
-        <v>539</v>
-      </c>
-      <c r="B202" t="s">
-        <v>233</v>
-      </c>
-      <c r="C202" t="s">
-        <v>232</v>
-      </c>
-      <c r="D202" t="s">
-        <v>228</v>
-      </c>
-      <c r="E202" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G202" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="B203" t="s">
-        <v>234</v>
+        <v>523</v>
       </c>
       <c r="C203" t="s">
-        <v>235</v>
+        <v>491</v>
       </c>
       <c r="D203" t="s">
-        <v>41</v>
+        <v>527</v>
       </c>
       <c r="E203" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="F203" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="G203" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="B204" t="s">
-        <v>236</v>
+        <v>524</v>
       </c>
       <c r="C204" t="s">
-        <v>237</v>
+        <v>492</v>
       </c>
       <c r="D204" t="s">
-        <v>238</v>
+        <v>527</v>
       </c>
       <c r="E204" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="F204" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="G204" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="B205" t="s">
-        <v>239</v>
+        <v>493</v>
       </c>
       <c r="C205" t="s">
-        <v>240</v>
+        <v>494</v>
       </c>
       <c r="D205" t="s">
-        <v>132</v>
+        <v>527</v>
       </c>
       <c r="E205" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="F205" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="B206" t="s">
-        <v>241</v>
+        <v>495</v>
       </c>
       <c r="C206" t="s">
-        <v>220</v>
+        <v>496</v>
       </c>
       <c r="D206" t="s">
-        <v>242</v>
+        <v>527</v>
       </c>
       <c r="E206" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="F206" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="B207" t="s">
-        <v>243</v>
+        <v>497</v>
       </c>
       <c r="C207" t="s">
-        <v>244</v>
+        <v>498</v>
       </c>
       <c r="D207" t="s">
-        <v>245</v>
+        <v>527</v>
       </c>
       <c r="E207" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="F207" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="B208" t="s">
-        <v>246</v>
+        <v>499</v>
       </c>
       <c r="C208" t="s">
-        <v>247</v>
+        <v>500</v>
       </c>
       <c r="D208" t="s">
-        <v>245</v>
+        <v>527</v>
       </c>
       <c r="E208" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="F208" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="B209" t="s">
-        <v>248</v>
+        <v>501</v>
       </c>
       <c r="C209" t="s">
-        <v>249</v>
+        <v>502</v>
       </c>
       <c r="D209" t="s">
-        <v>197</v>
+        <v>527</v>
       </c>
       <c r="E209" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+      <c r="F209" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="B210" t="s">
-        <v>250</v>
+        <v>503</v>
       </c>
       <c r="C210" t="s">
-        <v>251</v>
+        <v>504</v>
       </c>
       <c r="D210" t="s">
-        <v>252</v>
+        <v>527</v>
       </c>
       <c r="E210" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A211" t="s">
-        <v>539</v>
-      </c>
-      <c r="B211" t="s">
-        <v>253</v>
-      </c>
-      <c r="C211" t="s">
-        <v>251</v>
-      </c>
-      <c r="D211" t="s">
-        <v>252</v>
-      </c>
-      <c r="E211" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A212" t="s">
-        <v>539</v>
-      </c>
-      <c r="B212" t="s">
-        <v>254</v>
-      </c>
-      <c r="C212" t="s">
-        <v>255</v>
-      </c>
-      <c r="D212" t="s">
-        <v>197</v>
-      </c>
-      <c r="E212" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A213" t="s">
-        <v>539</v>
-      </c>
-      <c r="B213" t="s">
-        <v>256</v>
-      </c>
-      <c r="C213" t="s">
-        <v>257</v>
-      </c>
-      <c r="D213" t="s">
-        <v>245</v>
-      </c>
-      <c r="E213" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A214" t="s">
-        <v>539</v>
-      </c>
-      <c r="B214" t="s">
-        <v>258</v>
-      </c>
-      <c r="C214" t="s">
-        <v>259</v>
-      </c>
-      <c r="D214" t="s">
-        <v>260</v>
-      </c>
-      <c r="E214" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A215" t="s">
-        <v>539</v>
-      </c>
-      <c r="B215" t="s">
-        <v>261</v>
-      </c>
-      <c r="C215" t="s">
-        <v>259</v>
-      </c>
-      <c r="D215" t="s">
-        <v>262</v>
-      </c>
-      <c r="E215" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A216" t="s">
-        <v>539</v>
-      </c>
-      <c r="B216" t="s">
-        <v>263</v>
-      </c>
-      <c r="C216" t="s">
-        <v>264</v>
-      </c>
-      <c r="D216" t="s">
-        <v>43</v>
-      </c>
-      <c r="E216" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A217" t="s">
-        <v>539</v>
-      </c>
-      <c r="B217" t="s">
-        <v>265</v>
-      </c>
-      <c r="C217" t="s">
-        <v>266</v>
-      </c>
-      <c r="D217" t="s">
-        <v>267</v>
-      </c>
-      <c r="E217" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A218" t="s">
-        <v>539</v>
-      </c>
-      <c r="B218" t="s">
-        <v>268</v>
-      </c>
-      <c r="C218" t="s">
-        <v>264</v>
-      </c>
-      <c r="D218" t="s">
-        <v>269</v>
-      </c>
-      <c r="E218" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A219" t="s">
-        <v>539</v>
-      </c>
-      <c r="B219" t="s">
-        <v>270</v>
-      </c>
-      <c r="C219" t="s">
-        <v>271</v>
-      </c>
-      <c r="D219" t="s">
-        <v>272</v>
-      </c>
-      <c r="E219" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A220" t="s">
-        <v>539</v>
-      </c>
-      <c r="B220" t="s">
-        <v>273</v>
-      </c>
-      <c r="C220" t="s">
-        <v>274</v>
-      </c>
-      <c r="D220" t="s">
-        <v>41</v>
-      </c>
-      <c r="E220" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A221" t="s">
-        <v>539</v>
-      </c>
-      <c r="B221" t="s">
-        <v>275</v>
-      </c>
-      <c r="C221" t="s">
-        <v>286</v>
-      </c>
-      <c r="D221" t="s">
-        <v>276</v>
-      </c>
-      <c r="E221" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A222" t="s">
-        <v>539</v>
-      </c>
-      <c r="B222" t="s">
-        <v>277</v>
-      </c>
-      <c r="C222" t="s">
-        <v>278</v>
-      </c>
-      <c r="D222" t="s">
-        <v>279</v>
-      </c>
-      <c r="E222" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A223" t="s">
-        <v>539</v>
-      </c>
-      <c r="B223" t="s">
-        <v>280</v>
-      </c>
-      <c r="C223" t="s">
-        <v>281</v>
-      </c>
-      <c r="D223" t="s">
-        <v>197</v>
-      </c>
-      <c r="E223" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A224" t="s">
-        <v>539</v>
-      </c>
-      <c r="B224" t="s">
-        <v>282</v>
-      </c>
-      <c r="C224" t="s">
-        <v>283</v>
-      </c>
-      <c r="D224" t="s">
-        <v>284</v>
-      </c>
-      <c r="E224" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A225" t="s">
-        <v>539</v>
-      </c>
-      <c r="B225" t="s">
-        <v>287</v>
-      </c>
-      <c r="C225" t="s">
-        <v>288</v>
-      </c>
-      <c r="D225" t="s">
-        <v>228</v>
-      </c>
-      <c r="E225" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A226" t="s">
-        <v>539</v>
-      </c>
-      <c r="B226" t="s">
-        <v>289</v>
-      </c>
-      <c r="C226" t="s">
-        <v>290</v>
-      </c>
-      <c r="D226" t="s">
-        <v>228</v>
-      </c>
-      <c r="E226" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A227" t="s">
-        <v>539</v>
-      </c>
-      <c r="B227" t="s">
-        <v>291</v>
-      </c>
-      <c r="C227" t="s">
-        <v>292</v>
-      </c>
-      <c r="D227" t="s">
-        <v>41</v>
-      </c>
-      <c r="E227" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A228" t="s">
-        <v>539</v>
-      </c>
-      <c r="B228" t="s">
-        <v>293</v>
-      </c>
-      <c r="C228" t="s">
-        <v>294</v>
-      </c>
-      <c r="D228" t="s">
-        <v>245</v>
-      </c>
-      <c r="E228" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A229" t="s">
-        <v>539</v>
-      </c>
-      <c r="B229" t="s">
-        <v>295</v>
-      </c>
-      <c r="C229" t="s">
-        <v>296</v>
-      </c>
-      <c r="D229" t="s">
-        <v>41</v>
-      </c>
-      <c r="E229" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A230" t="s">
-        <v>539</v>
-      </c>
-      <c r="B230" t="s">
-        <v>297</v>
-      </c>
-      <c r="C230" t="s">
-        <v>298</v>
-      </c>
-      <c r="D230" t="s">
-        <v>197</v>
-      </c>
-      <c r="E230" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A231" t="s">
-        <v>539</v>
-      </c>
-      <c r="B231" t="s">
-        <v>299</v>
-      </c>
-      <c r="C231" t="s">
-        <v>300</v>
-      </c>
-      <c r="D231" t="s">
-        <v>301</v>
-      </c>
-      <c r="E231" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A232" t="s">
-        <v>539</v>
-      </c>
-      <c r="B232" t="s">
-        <v>302</v>
-      </c>
-      <c r="C232" t="s">
-        <v>303</v>
-      </c>
-      <c r="D232" t="s">
-        <v>301</v>
-      </c>
-      <c r="E232" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A233" t="s">
-        <v>539</v>
-      </c>
-      <c r="B233" t="s">
-        <v>304</v>
-      </c>
-      <c r="C233" t="s">
-        <v>305</v>
-      </c>
-      <c r="D233" t="s">
-        <v>306</v>
-      </c>
-      <c r="E233" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A234" t="s">
-        <v>539</v>
-      </c>
-      <c r="B234" t="s">
-        <v>307</v>
-      </c>
-      <c r="C234" t="s">
-        <v>308</v>
-      </c>
-      <c r="D234" t="s">
-        <v>41</v>
-      </c>
-      <c r="E234" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A235" t="s">
-        <v>528</v>
-      </c>
-      <c r="B235" t="s">
-        <v>460</v>
-      </c>
-      <c r="C235" t="s">
-        <v>461</v>
-      </c>
-      <c r="D235" t="s">
-        <v>529</v>
-      </c>
-      <c r="E235" t="s">
-        <v>40</v>
-      </c>
-      <c r="F235" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A236" t="s">
-        <v>528</v>
-      </c>
-      <c r="B236" t="s">
-        <v>462</v>
-      </c>
-      <c r="C236" t="s">
-        <v>463</v>
-      </c>
-      <c r="D236" t="s">
-        <v>529</v>
-      </c>
-      <c r="E236" t="s">
-        <v>40</v>
-      </c>
-      <c r="F236" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A237" t="s">
-        <v>528</v>
-      </c>
-      <c r="B237" t="s">
-        <v>464</v>
-      </c>
-      <c r="C237" t="s">
-        <v>465</v>
-      </c>
-      <c r="D237" t="s">
-        <v>529</v>
-      </c>
-      <c r="E237" t="s">
-        <v>40</v>
-      </c>
-      <c r="F237" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A238" t="s">
-        <v>528</v>
-      </c>
-      <c r="B238" t="s">
-        <v>466</v>
-      </c>
-      <c r="C238" t="s">
-        <v>467</v>
-      </c>
-      <c r="D238" t="s">
-        <v>529</v>
-      </c>
-      <c r="E238" t="s">
-        <v>40</v>
-      </c>
-      <c r="F238" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A239" t="s">
-        <v>528</v>
-      </c>
-      <c r="B239" t="s">
-        <v>468</v>
-      </c>
-      <c r="C239" t="s">
-        <v>469</v>
-      </c>
-      <c r="D239" t="s">
-        <v>529</v>
-      </c>
-      <c r="E239" t="s">
-        <v>40</v>
-      </c>
-      <c r="F239" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A240" t="s">
-        <v>528</v>
-      </c>
-      <c r="B240" t="s">
-        <v>390</v>
-      </c>
-      <c r="C240" t="s">
-        <v>470</v>
-      </c>
-      <c r="D240" t="s">
-        <v>529</v>
-      </c>
-      <c r="E240" t="s">
-        <v>40</v>
-      </c>
-      <c r="F240" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A241" t="s">
-        <v>528</v>
-      </c>
-      <c r="B241" t="s">
-        <v>471</v>
-      </c>
-      <c r="C241" t="s">
-        <v>472</v>
-      </c>
-      <c r="D241" t="s">
-        <v>529</v>
-      </c>
-      <c r="E241" t="s">
-        <v>40</v>
-      </c>
-      <c r="F241" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A242" t="s">
-        <v>528</v>
-      </c>
-      <c r="B242" t="s">
-        <v>473</v>
-      </c>
-      <c r="C242" t="s">
-        <v>474</v>
-      </c>
-      <c r="D242" t="s">
-        <v>529</v>
-      </c>
-      <c r="E242" t="s">
-        <v>40</v>
-      </c>
-      <c r="F242" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A243" t="s">
-        <v>528</v>
-      </c>
-      <c r="B243" t="s">
-        <v>475</v>
-      </c>
-      <c r="C243" t="s">
-        <v>476</v>
-      </c>
-      <c r="D243" t="s">
-        <v>529</v>
-      </c>
-      <c r="E243" t="s">
-        <v>40</v>
-      </c>
-      <c r="F243" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A244" t="s">
-        <v>528</v>
-      </c>
-      <c r="B244" t="s">
-        <v>477</v>
-      </c>
-      <c r="C244" t="s">
-        <v>478</v>
-      </c>
-      <c r="D244" t="s">
-        <v>529</v>
-      </c>
-      <c r="E244" t="s">
-        <v>40</v>
-      </c>
-      <c r="F244" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A245" t="s">
-        <v>528</v>
-      </c>
-      <c r="B245" t="s">
-        <v>479</v>
-      </c>
-      <c r="C245" t="s">
-        <v>480</v>
-      </c>
-      <c r="D245" t="s">
-        <v>529</v>
-      </c>
-      <c r="E245" t="s">
-        <v>40</v>
-      </c>
-      <c r="F245" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A246" t="s">
-        <v>528</v>
-      </c>
-      <c r="B246" t="s">
-        <v>481</v>
-      </c>
-      <c r="C246" t="s">
-        <v>482</v>
-      </c>
-      <c r="D246" t="s">
-        <v>529</v>
-      </c>
-      <c r="E246" t="s">
-        <v>40</v>
-      </c>
-      <c r="F246" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A247" t="s">
-        <v>528</v>
-      </c>
-      <c r="B247" t="s">
-        <v>483</v>
-      </c>
-      <c r="C247" t="s">
-        <v>484</v>
-      </c>
-      <c r="D247" t="s">
-        <v>529</v>
-      </c>
-      <c r="E247" t="s">
-        <v>40</v>
-      </c>
-      <c r="F247" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A248" t="s">
-        <v>528</v>
-      </c>
-      <c r="B248" t="s">
-        <v>485</v>
-      </c>
-      <c r="C248" t="s">
-        <v>486</v>
-      </c>
-      <c r="D248" t="s">
-        <v>529</v>
-      </c>
-      <c r="E248" t="s">
-        <v>40</v>
-      </c>
-      <c r="F248" s="1" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A249" t="s">
-        <v>528</v>
-      </c>
-      <c r="B249" t="s">
-        <v>487</v>
-      </c>
-      <c r="C249" t="s">
-        <v>488</v>
-      </c>
-      <c r="D249" t="s">
-        <v>529</v>
-      </c>
-      <c r="E249" t="s">
-        <v>40</v>
-      </c>
-      <c r="F249" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A250" t="s">
-        <v>528</v>
-      </c>
-      <c r="B250" t="s">
-        <v>489</v>
-      </c>
-      <c r="C250" t="s">
-        <v>490</v>
-      </c>
-      <c r="D250" t="s">
-        <v>529</v>
-      </c>
-      <c r="E250" t="s">
-        <v>40</v>
-      </c>
-      <c r="F250" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A251" t="s">
-        <v>528</v>
-      </c>
-      <c r="B251" t="s">
-        <v>524</v>
-      </c>
-      <c r="C251" t="s">
-        <v>491</v>
-      </c>
-      <c r="D251" t="s">
-        <v>529</v>
-      </c>
-      <c r="E251" t="s">
-        <v>40</v>
-      </c>
-      <c r="F251" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="G251" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A252" t="s">
-        <v>528</v>
-      </c>
-      <c r="B252" t="s">
-        <v>525</v>
-      </c>
-      <c r="C252" t="s">
-        <v>492</v>
-      </c>
-      <c r="D252" t="s">
-        <v>529</v>
-      </c>
-      <c r="E252" t="s">
-        <v>40</v>
-      </c>
-      <c r="F252" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="G252" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A253" t="s">
-        <v>528</v>
-      </c>
-      <c r="B253" t="s">
-        <v>526</v>
-      </c>
-      <c r="C253" t="s">
-        <v>493</v>
-      </c>
-      <c r="D253" t="s">
-        <v>529</v>
-      </c>
-      <c r="E253" t="s">
-        <v>40</v>
-      </c>
-      <c r="F253" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="G253" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A254" t="s">
-        <v>528</v>
-      </c>
-      <c r="B254" t="s">
-        <v>494</v>
-      </c>
-      <c r="C254" t="s">
-        <v>495</v>
-      </c>
-      <c r="D254" t="s">
-        <v>529</v>
-      </c>
-      <c r="E254" t="s">
-        <v>40</v>
-      </c>
-      <c r="F254" s="1" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A255" t="s">
-        <v>528</v>
-      </c>
-      <c r="B255" t="s">
-        <v>496</v>
-      </c>
-      <c r="C255" t="s">
-        <v>497</v>
-      </c>
-      <c r="D255" t="s">
-        <v>529</v>
-      </c>
-      <c r="E255" t="s">
-        <v>40</v>
-      </c>
-      <c r="F255" t="s">
+        <v>40</v>
+      </c>
+      <c r="F210" t="s">
         <v>521</v>
-      </c>
-    </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A256" t="s">
-        <v>528</v>
-      </c>
-      <c r="B256" t="s">
-        <v>498</v>
-      </c>
-      <c r="C256" t="s">
-        <v>499</v>
-      </c>
-      <c r="D256" t="s">
-        <v>529</v>
-      </c>
-      <c r="E256" t="s">
-        <v>40</v>
-      </c>
-      <c r="F256" s="1" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A257" t="s">
-        <v>528</v>
-      </c>
-      <c r="B257" t="s">
-        <v>500</v>
-      </c>
-      <c r="C257" t="s">
-        <v>501</v>
-      </c>
-      <c r="D257" t="s">
-        <v>529</v>
-      </c>
-      <c r="E257" t="s">
-        <v>40</v>
-      </c>
-      <c r="F257" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A258" t="s">
-        <v>528</v>
-      </c>
-      <c r="B258" t="s">
-        <v>502</v>
-      </c>
-      <c r="C258" t="s">
-        <v>503</v>
-      </c>
-      <c r="D258" t="s">
-        <v>529</v>
-      </c>
-      <c r="E258" t="s">
-        <v>40</v>
-      </c>
-      <c r="F258" s="1" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A259" t="s">
-        <v>528</v>
-      </c>
-      <c r="B259" t="s">
-        <v>504</v>
-      </c>
-      <c r="C259" t="s">
-        <v>505</v>
-      </c>
-      <c r="D259" t="s">
-        <v>529</v>
-      </c>
-      <c r="E259" t="s">
-        <v>40</v>
-      </c>
-      <c r="F259" t="s">
-        <v>523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>